<commit_message>
01032016 - Update Status Belum jalan
</commit_message>
<xml_diff>
--- a/list module.xlsx
+++ b/list module.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
   <si>
     <t>Login Form</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>List Jabatan</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +596,7 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
17032016 persiapan rapat dengan pak minto
</commit_message>
<xml_diff>
--- a/list module.xlsx
+++ b/list module.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>Login Form</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>List Jabatan</t>
-  </si>
-  <si>
-    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -489,7 +486,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,12 +593,15 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>